<commit_message>
Added Flow vs R1L to the cell data modeled by tissue slice  code
</commit_message>
<xml_diff>
--- a/Lac_AllBounds1.xlsx
+++ b/Lac_AllBounds1.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A03269-7003-43AD-89AE-6B3F33E2EAA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6426AC-58E6-40A4-859D-45465E88447A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{30AC0A47-4ED2-4AA0-BCC0-23EF3C1D9919}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{30AC0A47-4ED2-4AA0-BCC0-23EF3C1D9919}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>HK-2</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Kpl</t>
+  </si>
+  <si>
+    <t>Flow_Lac</t>
   </si>
 </sst>
 </file>
@@ -397,10 +400,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11FAE8E-12B5-45A2-96D7-7F3F6A71A4C5}">
-  <dimension ref="A1:J24"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:F24"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -970,6 +974,59 @@
         <v>4.3181921022227001E-3</v>
       </c>
     </row>
+    <row r="38" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <f>AVERAGE(F$1:F$3)</f>
+        <v>7.2733536860678421E-3</v>
+      </c>
+      <c r="H39">
+        <f>AVERAGE(F$4:F$6)</f>
+        <v>0.45917044925515804</v>
+      </c>
+      <c r="I39">
+        <f>AVERAGE(F$9:F$11)</f>
+        <v>0.67404326475165455</v>
+      </c>
+      <c r="J39">
+        <f>AVERAGE(F$13:F$16)</f>
+        <v>0.26571156370498145</v>
+      </c>
+    </row>
+    <row r="40" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <f>STDEV(F$1:F$3)/SQRT(COUNT(F$1:F$3))</f>
+        <v>7.2733422147735404E-3</v>
+      </c>
+      <c r="H40">
+        <f>STDEV(F$4:F$6)/SQRT(COUNT(F$4:F$6))</f>
+        <v>0.28055111686164436</v>
+      </c>
+      <c r="I40">
+        <f>STDEV(F$9:F$11)/SQRT(COUNT(F$9:F$11))</f>
+        <v>0.32595599527491059</v>
+      </c>
+      <c r="J40">
+        <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
+        <v>0.24488809179503482</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>